<commit_message>
Update grades from emails up to March 4
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 11 - Computer Architcture\CIS---11-Assembly-Programming\Work Tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Norco College\CIS 11 - Assembly Programming\CIS---11-Assembly-Programming\Work Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,12 +223,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,9 +250,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +572,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,20 +639,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
         <v>36</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>19</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>24</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
         <v>79</v>
       </c>
@@ -657,13 +664,22 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
       <c r="T3">
         <f t="shared" ref="T3:T43" si="0">SUM(C3:S3)</f>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="U3">
         <f>T3/T$2*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -673,13 +689,22 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0</v>
+        <v>1.0632911392405062</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -816,13 +841,16 @@
       <c r="E12">
         <v>19</v>
       </c>
+      <c r="F12">
+        <v>24</v>
+      </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.69620253164556967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -864,13 +892,16 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
+      <c r="D15">
+        <v>35</v>
+      </c>
       <c r="T15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44303797468354428</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1091,13 +1122,19 @@
       <c r="B29" t="s">
         <v>26</v>
       </c>
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>17</v>
+      </c>
       <c r="T29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.67088607594936711</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Grades up to 3/7.  Renamed week 4 and 5 work
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,13 +959,19 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
       <c r="T19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.67088607594936711</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -976,15 +982,21 @@
         <v>17</v>
       </c>
       <c r="D20">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
       </c>
       <c r="T20">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.45569620253164556</v>
+        <v>1.0632911392405062</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1042,13 +1054,22 @@
       <c r="B24" t="s">
         <v>21</v>
       </c>
+      <c r="D24">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <v>24</v>
+      </c>
       <c r="T24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1128,13 +1149,16 @@
       <c r="E29">
         <v>17</v>
       </c>
+      <c r="F29">
+        <v>24</v>
+      </c>
       <c r="T29">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.67088607594936711</v>
+        <v>0.97468354430379744</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1300,13 +1324,16 @@
       <c r="B39" t="s">
         <v>36</v>
       </c>
+      <c r="D39">
+        <v>41</v>
+      </c>
       <c r="T39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.51898734177215189</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add some assignment 6 grades
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -572,15 +572,18 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="7" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
@@ -653,11 +656,17 @@
         <v>24</v>
       </c>
       <c r="G2" s="2">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2">
+        <v>20</v>
       </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -677,7 +686,10 @@
         <v>24</v>
       </c>
       <c r="G3">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T43" si="0">SUM(C3:S3)</f>
@@ -685,7 +697,7 @@
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>1</v>
+        <v>0.83606557377049184</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -705,7 +717,10 @@
         <v>24</v>
       </c>
       <c r="G4">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
@@ -713,7 +728,7 @@
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>1.0490196078431373</v>
+        <v>0.87704918032786883</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -727,15 +742,21 @@
         <v>24</v>
       </c>
       <c r="G5">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.46078431372549017</v>
+        <v>0.54918032786885251</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -757,7 +778,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.58823529411764708</v>
+        <v>0.49180327868852458</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -809,7 +830,10 @@
         <v>24</v>
       </c>
       <c r="G9">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
@@ -817,7 +841,7 @@
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.83606557377049184</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -845,7 +869,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.84313725490196079</v>
+        <v>0.70491803278688525</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -886,7 +910,7 @@
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.77450980392156865</v>
+        <v>0.64754098360655743</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -905,7 +929,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.40196078431372551</v>
+        <v>0.33606557377049179</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -940,7 +964,7 @@
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.34313725490196079</v>
+        <v>0.28688524590163933</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1008,7 +1032,10 @@
         <v>23</v>
       </c>
       <c r="G19">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
       </c>
       <c r="T19">
         <f t="shared" si="0"/>
@@ -1016,7 +1043,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.97058823529411764</v>
+        <v>0.81147540983606559</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1036,7 +1063,10 @@
         <v>24</v>
       </c>
       <c r="G20">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
       </c>
       <c r="T20">
         <f t="shared" si="0"/>
@@ -1044,7 +1074,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>1.0392156862745099</v>
+        <v>0.86885245901639341</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1098,7 +1128,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.53921568627450978</v>
+        <v>0.45081967213114754</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1118,15 +1148,21 @@
         <v>24</v>
       </c>
       <c r="G24">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
       </c>
       <c r="T24">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.9509803921568627</v>
+        <v>0.91803278688524592</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1143,7 +1179,10 @@
         <v>24</v>
       </c>
       <c r="G25">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
       </c>
       <c r="T25">
         <f t="shared" si="0"/>
@@ -1151,7 +1190,7 @@
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.6470588235294118</v>
+        <v>0.54098360655737709</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1219,7 +1258,10 @@
         <v>24</v>
       </c>
       <c r="G29">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
       </c>
       <c r="T29">
         <f t="shared" si="0"/>
@@ -1227,7 +1269,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.98039215686274506</v>
+        <v>0.81967213114754101</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1249,7 +1291,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.57843137254901966</v>
+        <v>0.48360655737704916</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1367,7 +1409,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.58823529411764708</v>
+        <v>0.49180327868852458</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1403,7 +1445,10 @@
         <v>23</v>
       </c>
       <c r="G39">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="H39">
+        <v>10</v>
       </c>
       <c r="T39">
         <f t="shared" si="0"/>
@@ -1411,7 +1456,7 @@
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>1.0392156862745099</v>
+        <v>0.86885245901639341</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
lecture and assignment for week 8
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,9 +664,12 @@
       <c r="I2" s="2">
         <v>20</v>
       </c>
+      <c r="J2" s="2">
+        <v>20</v>
+      </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -697,7 +700,7 @@
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.83606557377049184</v>
+        <v>0.71830985915492962</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -728,7 +731,7 @@
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0.87704918032786883</v>
+        <v>0.75352112676056338</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -756,7 +759,7 @@
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.54918032786885251</v>
+        <v>0.47183098591549294</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -778,7 +781,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.49180327868852458</v>
+        <v>0.42253521126760563</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -788,13 +791,34 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0352112676056338</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -835,13 +859,16 @@
       <c r="H9">
         <v>10</v>
       </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>0.83606557377049184</v>
+        <v>0.85915492957746475</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -869,7 +896,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.70491803278688525</v>
+        <v>0.60563380281690138</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -879,13 +906,16 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
       <c r="T11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.23239436619718309</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -910,7 +940,7 @@
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.64754098360655743</v>
+        <v>0.55633802816901412</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -929,7 +959,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.33606557377049179</v>
+        <v>0.28873239436619719</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -964,7 +994,7 @@
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.28688524590163933</v>
+        <v>0.24647887323943662</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1006,13 +1036,28 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
+      <c r="D18">
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+      <c r="F18">
+        <v>24</v>
+      </c>
+      <c r="G18">
+        <v>13</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75352112676056338</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
@@ -1043,7 +1088,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.81147540983606559</v>
+        <v>0.69718309859154926</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1074,7 +1119,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.86885245901639341</v>
+        <v>0.74647887323943662</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1128,7 +1173,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.45081967213114754</v>
+        <v>0.38732394366197181</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1162,7 +1207,7 @@
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.91803278688524592</v>
+        <v>0.78873239436619713</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1190,7 +1235,7 @@
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.54098360655737709</v>
+        <v>0.46478873239436619</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1269,7 +1314,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.81967213114754101</v>
+        <v>0.70422535211267601</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1291,7 +1336,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.48360655737704916</v>
+        <v>0.41549295774647887</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1409,7 +1454,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.49180327868852458</v>
+        <v>0.42253521126760563</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1456,7 +1501,7 @@
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.86885245901639341</v>
+        <v>0.74647887323943662</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update grades through 4/11
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,9 +667,12 @@
       <c r="J2" s="2">
         <v>20</v>
       </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -700,7 +703,7 @@
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.71830985915492962</v>
+        <v>0.69863013698630139</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -725,13 +728,16 @@
       <c r="H4">
         <v>10</v>
       </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0.75352112676056338</v>
+        <v>0.79452054794520544</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -753,13 +759,16 @@
       <c r="I5">
         <v>20</v>
       </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.47183098591549294</v>
+        <v>0.52054794520547942</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -781,7 +790,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.42253521126760563</v>
+        <v>0.41095890410958902</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -812,13 +821,16 @@
       <c r="J7">
         <v>20</v>
       </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>1.0352112676056338</v>
+        <v>1.0684931506849316</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -862,13 +874,19 @@
       <c r="I9">
         <v>20</v>
       </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>0.85915492957746475</v>
+        <v>1.0342465753424657</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -896,7 +914,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.60563380281690138</v>
+        <v>0.58904109589041098</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -915,7 +933,7 @@
       </c>
       <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>0.23239436619718309</v>
+        <v>0.22602739726027396</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -934,13 +952,22 @@
       <c r="F12">
         <v>24</v>
       </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.55633802816901412</v>
+        <v>0.83561643835616439</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -959,7 +986,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.28873239436619719</v>
+        <v>0.28082191780821919</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -988,13 +1015,16 @@
       <c r="D15">
         <v>35</v>
       </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
       <c r="T15">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.24647887323943662</v>
+        <v>0.36986301369863012</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1004,13 +1034,22 @@
       <c r="B16" t="s">
         <v>13</v>
       </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
       <c r="T16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.53424657534246578</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -1051,13 +1090,16 @@
       <c r="H18">
         <v>10</v>
       </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>0.75352112676056338</v>
+        <v>0.79452054794520544</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
@@ -1088,7 +1130,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.69718309859154926</v>
+        <v>0.67808219178082196</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1119,7 +1161,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.74647887323943662</v>
+        <v>0.72602739726027399</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1167,13 +1209,22 @@
       <c r="E23">
         <v>19</v>
       </c>
+      <c r="F23">
+        <v>24</v>
+      </c>
+      <c r="G23">
+        <v>13</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
       <c r="T23">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.38732394366197181</v>
+        <v>0.69863013698630139</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1199,15 +1250,18 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="K24">
+        <v>9</v>
       </c>
       <c r="T24">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.78873239436619713</v>
+        <v>0.89726027397260277</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1217,6 +1271,9 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
+      <c r="D25">
+        <v>40</v>
+      </c>
       <c r="E25">
         <v>19</v>
       </c>
@@ -1229,13 +1286,16 @@
       <c r="H25">
         <v>10</v>
       </c>
+      <c r="K25">
+        <v>9</v>
+      </c>
       <c r="T25">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.46478873239436619</v>
+        <v>0.78767123287671237</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1314,7 +1374,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.70422535211267601</v>
+        <v>0.68493150684931503</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1336,7 +1396,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.41549295774647887</v>
+        <v>0.4041095890410959</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1454,7 +1514,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.42253521126760563</v>
+        <v>0.41095890410958902</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1464,13 +1524,22 @@
       <c r="B38" t="s">
         <v>35</v>
       </c>
+      <c r="E38">
+        <v>19</v>
+      </c>
+      <c r="G38">
+        <v>13</v>
+      </c>
+      <c r="H38">
+        <v>10</v>
+      </c>
       <c r="T38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28767123287671231</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -1501,7 +1570,7 @@
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.74647887323943662</v>
+        <v>0.72602739726027399</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update some grades.  Update 32 bit solution file
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -250,10 +250,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +574,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,9 +672,15 @@
       <c r="K2" s="2">
         <v>4</v>
       </c>
+      <c r="L2" s="2">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>146</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -703,7 +711,7 @@
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.69863013698630139</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -737,7 +745,7 @@
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0.79452054794520544</v>
+        <v>0.69047619047619047</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -768,7 +776,7 @@
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.52054794520547942</v>
+        <v>0.45238095238095238</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -790,7 +798,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.41095890410958902</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -830,7 +838,7 @@
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>1.0684931506849316</v>
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -886,7 +894,7 @@
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>1.0342465753424657</v>
+        <v>0.89880952380952384</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -914,26 +922,44 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.58904109589041098</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11">
+        <v>0.51190476190476186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
         <v>2492435</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>33</v>
       </c>
-      <c r="T11">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="U11" s="1">
-        <f t="shared" si="1"/>
-        <v>0.22602739726027396</v>
+      <c r="F11" s="3">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3">
+        <v>13</v>
+      </c>
+      <c r="H11" s="3">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3">
+        <v>20</v>
+      </c>
+      <c r="J11" s="3">
+        <v>20</v>
+      </c>
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="T11" s="3">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.72619047619047616</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -958,16 +984,22 @@
       <c r="H12">
         <v>10</v>
       </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
       <c r="J12">
         <v>20</v>
       </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.83561643835616439</v>
+        <v>0.89880952380952384</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -986,7 +1018,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.28082191780821919</v>
+        <v>0.24404761904761904</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -1024,7 +1056,7 @@
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.36986301369863012</v>
+        <v>0.32142857142857145</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1049,7 +1081,7 @@
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>0.53424657534246578</v>
+        <v>0.4642857142857143</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -1090,16 +1122,19 @@
       <c r="H18">
         <v>10</v>
       </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
       <c r="K18">
         <v>9</v>
       </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>0.79452054794520544</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
@@ -1130,7 +1165,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.67808219178082196</v>
+        <v>0.5892857142857143</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1161,7 +1196,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.72602739726027399</v>
+        <v>0.63095238095238093</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1224,7 +1259,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.69863013698630139</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1261,7 +1296,7 @@
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.89726027397260277</v>
+        <v>0.77976190476190477</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1295,7 +1330,7 @@
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.78767123287671237</v>
+        <v>0.68452380952380953</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1374,7 +1409,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.68493150684931503</v>
+        <v>0.59523809523809523</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1396,7 +1431,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.4041095890410959</v>
+        <v>0.35119047619047616</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1514,7 +1549,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.41095890410958902</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1539,7 +1574,7 @@
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0.28767123287671231</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -1564,13 +1599,16 @@
       <c r="H39">
         <v>10</v>
       </c>
+      <c r="I39">
+        <v>20</v>
+      </c>
       <c r="T39">
         <f t="shared" si="0"/>
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.72602739726027399</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
@@ -1628,13 +1666,22 @@
       <c r="B43" t="s">
         <v>40</v>
       </c>
+      <c r="D43">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>18</v>
+      </c>
+      <c r="F43">
+        <v>24</v>
+      </c>
       <c r="T43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="U43" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.49404761904761907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update grades up to 5/6
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -574,7 +574,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,9 +678,12 @@
       <c r="M2" s="2">
         <v>0</v>
       </c>
+      <c r="N2" s="2">
+        <v>22</v>
+      </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -705,13 +708,22 @@
       <c r="H3">
         <v>10</v>
       </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
       <c r="T3">
         <f t="shared" ref="T3:T43" si="0">SUM(C3:S3)</f>
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.6071428571428571</v>
+        <v>0.66842105263157892</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -745,7 +757,7 @@
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0.69047619047619047</v>
+        <v>0.61052631578947369</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -776,7 +788,7 @@
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.45238095238095238</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -798,7 +810,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.35714285714285715</v>
+        <v>0.31578947368421051</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -832,13 +844,19 @@
       <c r="K7">
         <v>9</v>
       </c>
+      <c r="L7">
+        <v>22</v>
+      </c>
+      <c r="N7">
+        <v>22</v>
+      </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>0.9285714285714286</v>
+        <v>1.0526315789473684</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -894,7 +912,7 @@
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>0.89880952380952384</v>
+        <v>0.79473684210526319</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -922,7 +940,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.51190476190476186</v>
+        <v>0.45263157894736844</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -953,13 +971,16 @@
       <c r="K11" s="3">
         <v>4</v>
       </c>
+      <c r="N11" s="3">
+        <v>22</v>
+      </c>
       <c r="T11" s="3">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" si="1"/>
-        <v>0.72619047619047616</v>
+        <v>0.75789473684210529</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -999,7 +1020,7 @@
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.89880952380952384</v>
+        <v>0.79473684210526319</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -1012,13 +1033,19 @@
       <c r="D13">
         <v>41</v>
       </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>24</v>
+      </c>
       <c r="T13">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.24404761904761904</v>
+        <v>0.44210526315789472</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -1050,13 +1077,19 @@
       <c r="E15">
         <v>19</v>
       </c>
+      <c r="I15">
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
       <c r="T15">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.32142857142857145</v>
+        <v>0.41578947368421054</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1081,7 +1114,7 @@
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>0.4642857142857143</v>
+        <v>0.41052631578947368</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -1128,13 +1161,19 @@
       <c r="K18">
         <v>9</v>
       </c>
+      <c r="L18">
+        <v>22</v>
+      </c>
+      <c r="N18">
+        <v>22</v>
+      </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>0.80952380952380953</v>
+        <v>0.94736842105263153</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
@@ -1165,7 +1204,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.5892857142857143</v>
+        <v>0.52105263157894732</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1196,7 +1235,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.63095238095238093</v>
+        <v>0.55789473684210522</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1259,7 +1298,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.6071428571428571</v>
+        <v>0.5368421052631579</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1287,16 +1326,22 @@
       <c r="I24">
         <v>20</v>
       </c>
+      <c r="J24">
+        <v>20</v>
+      </c>
       <c r="K24">
         <v>9</v>
       </c>
+      <c r="N24">
+        <v>22</v>
+      </c>
       <c r="T24">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.77976190476190477</v>
+        <v>0.91052631578947374</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1321,16 +1366,22 @@
       <c r="H25">
         <v>10</v>
       </c>
+      <c r="I25">
+        <v>20</v>
+      </c>
       <c r="K25">
         <v>9</v>
       </c>
+      <c r="N25">
+        <v>22</v>
+      </c>
       <c r="T25">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.68452380952380953</v>
+        <v>0.82631578947368423</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1409,7 +1460,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.59523809523809523</v>
+        <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1431,7 +1482,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.35119047619047616</v>
+        <v>0.31052631578947371</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1543,13 +1594,19 @@
       <c r="E37">
         <v>19</v>
       </c>
+      <c r="F37">
+        <v>24</v>
+      </c>
+      <c r="G37">
+        <v>13</v>
+      </c>
       <c r="T37">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.35714285714285715</v>
+        <v>0.51052631578947372</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1568,13 +1625,16 @@
       <c r="H38">
         <v>10</v>
       </c>
+      <c r="N38">
+        <v>22</v>
+      </c>
       <c r="T38">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.33684210526315789</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -1602,13 +1662,16 @@
       <c r="I39">
         <v>20</v>
       </c>
+      <c r="J39">
+        <v>20</v>
+      </c>
       <c r="T39">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.76842105263157889</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
@@ -1681,7 +1744,7 @@
       </c>
       <c r="U43" s="1">
         <f t="shared" si="1"/>
-        <v>0.49404761904761907</v>
+        <v>0.43684210526315792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish grades up to 5/6
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -207,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,8 +222,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +243,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -246,18 +259,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -573,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +599,8 @@
     <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
@@ -616,7 +633,7 @@
       <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>51</v>
       </c>
       <c r="N1" t="s">
@@ -675,7 +692,7 @@
       <c r="L2" s="2">
         <v>22</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="5">
         <v>0</v>
       </c>
       <c r="N2" s="2">
@@ -708,6 +725,9 @@
       <c r="H3">
         <v>10</v>
       </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
       <c r="J3">
         <v>10</v>
       </c>
@@ -719,11 +739,11 @@
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T43" si="0">SUM(C3:S3)</f>
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.66842105263157892</v>
+        <v>0.77368421052631575</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -779,16 +799,19 @@
       <c r="I5">
         <v>20</v>
       </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
       <c r="K5">
         <v>9</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.4</v>
+        <v>0.50526315789473686</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -906,13 +929,16 @@
       <c r="K9">
         <v>9</v>
       </c>
+      <c r="L9">
+        <v>22</v>
+      </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>0.79473684210526319</v>
+        <v>0.91052631578947374</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -934,13 +960,22 @@
       <c r="G10">
         <v>13</v>
       </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
       <c r="T10">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.45263157894736844</v>
+        <v>0.63157894736842102</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -971,6 +1006,7 @@
       <c r="K11" s="3">
         <v>4</v>
       </c>
+      <c r="M11" s="5"/>
       <c r="N11" s="3">
         <v>22</v>
       </c>
@@ -1014,13 +1050,16 @@
       <c r="K12">
         <v>9</v>
       </c>
+      <c r="L12">
+        <v>22</v>
+      </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.79473684210526319</v>
+        <v>0.91052631578947374</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -1077,19 +1116,31 @@
       <c r="E15">
         <v>19</v>
       </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
       <c r="I15">
         <v>20</v>
       </c>
       <c r="J15">
         <v>5</v>
       </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
       <c r="T15">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.41578947368421054</v>
+        <v>0.68421052631578949</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1476,13 +1527,28 @@
       <c r="E30">
         <v>19</v>
       </c>
+      <c r="F30">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
       <c r="T30">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.31052631578947371</v>
+        <v>0.64736842105263159</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1625,16 +1691,19 @@
       <c r="H38">
         <v>10</v>
       </c>
+      <c r="L38">
+        <v>22</v>
+      </c>
       <c r="N38">
         <v>22</v>
       </c>
       <c r="T38">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0.33684210526315789</v>
+        <v>0.45263157894736844</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -1738,13 +1807,16 @@
       <c r="F43">
         <v>24</v>
       </c>
+      <c r="K43">
+        <v>5</v>
+      </c>
       <c r="T43">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="U43" s="1">
         <f t="shared" si="1"/>
-        <v>0.43684210526315792</v>
+        <v>0.4631578947368421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Most grades are complete
</commit_message>
<xml_diff>
--- a/Work Tracking/Grades.xlsx
+++ b/Work Tracking/Grades.xlsx
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,9 +698,24 @@
       <c r="N2" s="2">
         <v>22</v>
       </c>
+      <c r="O2" s="2">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
       <c r="T2" s="2">
         <f>SUM(C2:S2)</f>
-        <v>190</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -729,7 +744,7 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -737,13 +752,22 @@
       <c r="L3">
         <v>11</v>
       </c>
+      <c r="N3">
+        <v>22</v>
+      </c>
+      <c r="O3">
+        <v>25</v>
+      </c>
+      <c r="P3">
+        <v>25</v>
+      </c>
       <c r="T3">
         <f t="shared" ref="T3:T43" si="0">SUM(C3:S3)</f>
-        <v>147</v>
+        <v>229</v>
       </c>
       <c r="U3" s="1">
         <f>T3/T$2</f>
-        <v>0.77368421052631575</v>
+        <v>0.95416666666666672</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -777,7 +801,7 @@
       </c>
       <c r="U4" s="1">
         <f>T4/T$2</f>
-        <v>0.61052631578947369</v>
+        <v>0.48333333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -808,13 +832,22 @@
       <c r="K5">
         <v>9</v>
       </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>22</v>
+      </c>
+      <c r="P5">
+        <v>13</v>
+      </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" ref="U5:U43" si="1">T5/T$2</f>
-        <v>0.72105263157894739</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -836,7 +869,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>0.31578947368421051</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -882,7 +915,7 @@
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>1.0526315789473684</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -935,13 +968,19 @@
       <c r="L9">
         <v>22</v>
       </c>
+      <c r="O9">
+        <v>25</v>
+      </c>
+      <c r="P9">
+        <v>25</v>
+      </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>0.91052631578947374</v>
+        <v>0.9291666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -972,13 +1011,22 @@
       <c r="K10">
         <v>4</v>
       </c>
+      <c r="L10">
+        <v>20</v>
+      </c>
+      <c r="N10">
+        <v>22</v>
+      </c>
+      <c r="P10">
+        <v>25</v>
+      </c>
       <c r="T10">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>187</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>0.63157894736842102</v>
+        <v>0.77916666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1019,7 +1067,7 @@
       </c>
       <c r="U11" s="4">
         <f t="shared" si="1"/>
-        <v>0.75789473684210529</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -1056,13 +1104,22 @@
       <c r="L12">
         <v>22</v>
       </c>
+      <c r="N12">
+        <v>22</v>
+      </c>
+      <c r="O12">
+        <v>25</v>
+      </c>
+      <c r="P12">
+        <v>25</v>
+      </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>173</v>
+        <v>245</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>0.91052631578947374</v>
+        <v>1.0208333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -1081,13 +1138,28 @@
       <c r="F13">
         <v>24</v>
       </c>
+      <c r="G13">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>22</v>
+      </c>
       <c r="T13">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>0.44210526315789472</v>
+        <v>0.70416666666666672</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -1097,13 +1169,34 @@
       <c r="B14" t="s">
         <v>11</v>
       </c>
+      <c r="D14">
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
       <c r="T14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="U14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.54583333333333328</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
@@ -1143,7 +1236,7 @@
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>0.68421052631578949</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1168,7 +1261,7 @@
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>0.41052631578947368</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -1221,13 +1314,16 @@
       <c r="N18">
         <v>22</v>
       </c>
+      <c r="P18">
+        <v>25</v>
+      </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
+        <v>0.85416666666666663</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
@@ -1238,7 +1334,7 @@
         <v>16</v>
       </c>
       <c r="D19">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E19">
         <v>19</v>
@@ -1252,13 +1348,22 @@
       <c r="H19">
         <v>10</v>
       </c>
+      <c r="I19">
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>15</v>
+      </c>
       <c r="T19">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>0.52105263157894732</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -1289,7 +1394,7 @@
       </c>
       <c r="U20" s="1">
         <f t="shared" si="1"/>
-        <v>0.55789473684210522</v>
+        <v>0.44166666666666665</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
@@ -1352,7 +1457,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>0.5368421052631579</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
@@ -1395,7 +1500,7 @@
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>0.91052631578947374</v>
+        <v>0.72083333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
@@ -1429,13 +1534,16 @@
       <c r="N25">
         <v>22</v>
       </c>
+      <c r="O25">
+        <v>25</v>
+      </c>
       <c r="T25">
         <f t="shared" si="0"/>
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>0.82631578947368423</v>
+        <v>0.7583333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
@@ -1477,13 +1585,49 @@
       <c r="B28" t="s">
         <v>25</v>
       </c>
+      <c r="D28">
+        <v>41</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>13</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>20</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>22</v>
+      </c>
+      <c r="N28">
+        <v>22</v>
+      </c>
+      <c r="O28">
+        <v>25</v>
+      </c>
+      <c r="P28">
+        <v>25</v>
+      </c>
       <c r="T28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="U28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0208333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
@@ -1508,13 +1652,25 @@
       <c r="H29">
         <v>10</v>
       </c>
+      <c r="I29">
+        <v>20</v>
+      </c>
+      <c r="N29">
+        <v>22</v>
+      </c>
+      <c r="O29">
+        <v>25</v>
+      </c>
+      <c r="P29">
+        <v>25</v>
+      </c>
       <c r="T29">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>0.52631578947368418</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
@@ -1536,8 +1692,11 @@
       <c r="G30">
         <v>13</v>
       </c>
+      <c r="H30">
+        <v>10</v>
+      </c>
       <c r="I30">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J30">
         <v>20</v>
@@ -1545,13 +1704,25 @@
       <c r="K30">
         <v>4</v>
       </c>
+      <c r="L30">
+        <v>22</v>
+      </c>
+      <c r="N30">
+        <v>22</v>
+      </c>
+      <c r="O30">
+        <v>25</v>
+      </c>
+      <c r="P30">
+        <v>25</v>
+      </c>
       <c r="T30">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>0.64736842105263159</v>
+        <v>1.0166666666666666</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
@@ -1675,7 +1846,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>0.51052631578947372</v>
+        <v>0.40416666666666667</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
@@ -1694,6 +1865,9 @@
       <c r="H38">
         <v>10</v>
       </c>
+      <c r="I38">
+        <v>20</v>
+      </c>
       <c r="L38">
         <v>22</v>
       </c>
@@ -1702,11 +1876,11 @@
       </c>
       <c r="T38">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0.45263157894736844</v>
+        <v>0.44166666666666665</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
@@ -1743,7 +1917,7 @@
       </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.76842105263157889</v>
+        <v>0.60833333333333328</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.35">
@@ -1810,16 +1984,40 @@
       <c r="F43">
         <v>24</v>
       </c>
+      <c r="G43">
+        <v>13</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="I43">
+        <v>20</v>
+      </c>
+      <c r="J43">
+        <v>20</v>
+      </c>
       <c r="K43">
         <v>5</v>
       </c>
+      <c r="L43">
+        <v>22</v>
+      </c>
+      <c r="N43">
+        <v>22</v>
+      </c>
+      <c r="O43">
+        <v>25</v>
+      </c>
+      <c r="P43">
+        <v>25</v>
+      </c>
       <c r="T43">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>245</v>
       </c>
       <c r="U43" s="1">
         <f t="shared" si="1"/>
-        <v>0.4631578947368421</v>
+        <v>1.0208333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>